<commit_message>
Auto-committed on 2021/12/06 週一
Former-commit-id: 23ef3d30f0d77bbae2b0a42869aee795e448dd7f
</commit_message>
<xml_diff>
--- a/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/SystemParas.xlsx
+++ b/Program/Other/URS會議審查紀錄/DbLayouts/L6-共同作業/SystemParas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SKL\DB\GenTables\L6-共同作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7E665E-FF3C-4923-992B-867A7346408D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE90A01E-F1CF-4C27-8112-BADF08369DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="232">
   <si>
     <t>讀取Key條件</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -941,6 +941,17 @@
   <si>
     <t>單筆預收期數</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmpNoList</t>
+  </si>
+  <si>
+    <t>業績追回通知員工代碼清單</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L6501維護 add 2021/12/6 by 智誠
+預設空白</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1150,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1256,6 +1267,9 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1596,10 +1610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2206,7 +2220,7 @@
     </row>
     <row r="31" spans="1:7" ht="64.8" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
-        <f t="shared" ref="A31:A34" si="2">A30+1</f>
+        <f t="shared" ref="A31:A35" si="2">A30+1</f>
         <v>23</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -2250,36 +2264,36 @@
     </row>
     <row r="33" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
-        <f t="shared" si="2"/>
+        <f>A32+1</f>
         <v>25</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="19">
-        <v>3</v>
-      </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="22" t="s">
-        <v>223</v>
+      <c r="B33" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="28">
+        <v>150</v>
+      </c>
+      <c r="F33" s="28"/>
+      <c r="G33" s="39" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
-        <f t="shared" si="2"/>
+        <f>A33+1</f>
         <v>26</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>95</v>
@@ -2289,19 +2303,19 @@
       </c>
       <c r="F34" s="19"/>
       <c r="G34" s="22" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <f t="shared" ref="A35:A39" si="3">A34+1</f>
         <v>27</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>95</v>
@@ -2320,10 +2334,10 @@
         <v>28</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>95</v>
@@ -2333,19 +2347,19 @@
       </c>
       <c r="F36" s="19"/>
       <c r="G36" s="22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>95</v>
@@ -2358,16 +2372,16 @@
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>95</v>
@@ -2377,29 +2391,29 @@
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="22" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>95</v>
       </c>
       <c r="E39" s="19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F39" s="19"/>
       <c r="G39" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -2408,20 +2422,20 @@
         <v>32</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>228</v>
+        <v>165</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>162</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>95</v>
       </c>
       <c r="E40" s="19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F40" s="19"/>
       <c r="G40" s="22" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -2430,10 +2444,10 @@
         <v>33</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="C41" s="36" t="s">
-        <v>227</v>
+        <v>164</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>228</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>95</v>
@@ -2442,6 +2456,9 @@
         <v>3</v>
       </c>
       <c r="F41" s="19"/>
+      <c r="G41" s="22" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="42" spans="1:7" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
@@ -2449,10 +2466,10 @@
         <v>34</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>168</v>
+        <v>226</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>227</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>95</v>
@@ -2461,7 +2478,6 @@
         <v>3</v>
       </c>
       <c r="F42" s="19"/>
-      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="1:7" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
@@ -2469,10 +2485,10 @@
         <v>35</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D43" s="19" t="s">
         <v>95</v>
@@ -2483,26 +2499,24 @@
       <c r="F43" s="19"/>
       <c r="G43" s="22"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27">
         <v>36</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D44" s="19" t="s">
         <v>95</v>
       </c>
       <c r="E44" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F44" s="19"/>
-      <c r="G44" s="22" t="s">
-        <v>183</v>
-      </c>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
@@ -2510,19 +2524,21 @@
         <v>37</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>175</v>
+        <v>95</v>
       </c>
       <c r="E45" s="19">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F45" s="19"/>
-      <c r="G45" s="22"/>
+      <c r="G45" s="22" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
@@ -2530,41 +2546,39 @@
         <v>38</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>30</v>
+        <v>174</v>
       </c>
       <c r="D46" s="19" t="s">
-        <v>32</v>
+        <v>175</v>
       </c>
       <c r="E46" s="19">
-        <v>8</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>132</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F46" s="19"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <f t="shared" si="4"/>
         <v>39</v>
       </c>
-      <c r="B47" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="29">
-        <v>3</v>
-      </c>
-      <c r="F47" s="30"/>
-      <c r="G47" s="31" t="s">
-        <v>208</v>
+      <c r="B47" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="19">
+        <v>8</v>
+      </c>
+      <c r="G47" s="21" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2573,10 +2587,10 @@
         <v>40</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D48" s="29" t="s">
         <v>18</v>
@@ -2586,7 +2600,7 @@
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2594,21 +2608,21 @@
         <f t="shared" si="4"/>
         <v>41</v>
       </c>
-      <c r="B49" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="19">
-        <v>8</v>
-      </c>
-      <c r="F49" s="19"/>
-      <c r="G49" s="22" t="s">
-        <v>131</v>
+      <c r="B49" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="29">
+        <v>3</v>
+      </c>
+      <c r="F49" s="30"/>
+      <c r="G49" s="31" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2616,21 +2630,21 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="B50" s="29" t="s">
-        <v>216</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>217</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>218</v>
-      </c>
-      <c r="E50" s="29">
-        <v>1</v>
-      </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="35" t="s">
-        <v>219</v>
+      <c r="B50" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="19">
+        <v>8</v>
+      </c>
+      <c r="F50" s="19"/>
+      <c r="G50" s="22" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2638,21 +2652,21 @@
         <f t="shared" si="4"/>
         <v>43</v>
       </c>
-      <c r="B51" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D51" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="E51" s="33">
-        <v>100</v>
-      </c>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34" t="s">
-        <v>214</v>
+      <c r="B51" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="E51" s="29">
+        <v>1</v>
+      </c>
+      <c r="F51" s="29"/>
+      <c r="G51" s="35" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2661,20 +2675,20 @@
         <v>44</v>
       </c>
       <c r="B52" s="33" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C52" s="33" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D52" s="33" t="s">
-        <v>105</v>
+        <v>215</v>
       </c>
       <c r="E52" s="33">
         <v>100</v>
       </c>
       <c r="F52" s="33"/>
       <c r="G52" s="34" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2682,18 +2696,22 @@
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="B53" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="22"/>
+      <c r="B53" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="33">
+        <v>100</v>
+      </c>
+      <c r="F53" s="33"/>
+      <c r="G53" s="34" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="32">
@@ -2701,17 +2719,15 @@
         <v>46</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="19">
-        <v>6</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E54" s="19"/>
       <c r="F54" s="19"/>
       <c r="G54" s="22"/>
     </row>
@@ -2721,15 +2737,17 @@
         <v>47</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55" s="19"/>
+        <v>18</v>
+      </c>
+      <c r="E55" s="19">
+        <v>6</v>
+      </c>
       <c r="F55" s="19"/>
       <c r="G55" s="22"/>
     </row>
@@ -2739,30 +2757,38 @@
         <v>48</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="19">
-        <v>6</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E56" s="19"/>
       <c r="F56" s="19"/>
       <c r="G56" s="22"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
+      <c r="A57" s="4">
+        <v>49</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="19">
+        <v>6</v>
+      </c>
       <c r="F57" s="19"/>
       <c r="G57" s="22"/>
     </row>
-    <row r="58" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
@@ -2771,7 +2797,7 @@
       <c r="F58" s="19"/>
       <c r="G58" s="22"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
@@ -2851,6 +2877,15 @@
       <c r="E67" s="19"/>
       <c r="F67" s="19"/>
       <c r="G67" s="22"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>